<commit_message>
done on a Friday afternoon
</commit_message>
<xml_diff>
--- a/analysis/supplementary-materials/Table 8 of Porter et al 2022 RT.xlsx
+++ b/analysis/supplementary-materials/Table 8 of Porter et al 2022 RT.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mikea\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\DeadwaterPaper\analysis\supplementary-materials\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E58506FD-1B1A-42AC-ABE5-BC7714828D70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A49DAE0-226D-458A-8656-AEC08040C793}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B94EB891-2A36-48F2-87D6-9BC7BB5FB8B3}"/>
   </bookViews>
@@ -35,6 +35,24 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={42FFB360-E246-4651-AC14-22D7EE52F34B}</author>
+  </authors>
+  <commentList>
+    <comment ref="D18" authorId="0" shapeId="0" xr:uid="{42FFB360-E246-4651-AC14-22D7EE52F34B}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    BY2018 from McClure et al. 2021</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -71,7 +89,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -93,6 +111,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -164,6 +188,9 @@
     <xf numFmtId="3" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -172,9 +199,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -191,6 +215,12 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="Mike Ackerman" id="{EBE2739B-2F35-49AF-9A3C-64870814F63D}" userId="Mike Ackerman" providerId="None"/>
+</personList>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -488,12 +518,20 @@
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="D18" dT="2022-04-01T19:43:11.93" personId="{EBE2739B-2F35-49AF-9A3C-64870814F63D}" id="{42FFB360-E246-4651-AC14-22D7EE52F34B}">
+    <text>BY2018 from McClure et al. 2021</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB40FE9C-B375-457C-8A47-9739703F7EA8}">
-  <dimension ref="B1:I13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB40FE9C-B375-457C-8A47-9739703F7EA8}">
+  <dimension ref="B1:I18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -506,23 +544,23 @@
   <sheetData>
     <row r="1" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9" t="s">
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="H2" s="9"/>
-      <c r="I2" s="9"/>
+      <c r="H2" s="10"/>
+      <c r="I2" s="10"/>
     </row>
     <row r="3" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="8"/>
+      <c r="B3" s="9"/>
       <c r="C3" s="1" t="s">
         <v>3</v>
       </c>
@@ -731,23 +769,31 @@
       <c r="B11" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="10">
+      <c r="C11" s="7">
         <f>AVERAGE(C4:C10)</f>
         <v>806.42857142857144</v>
       </c>
-      <c r="D11" s="10">
-        <f t="shared" ref="D11:E11" si="0">AVERAGE(D4:D10)</f>
+      <c r="D11" s="7">
+        <f t="shared" ref="D11" si="0">AVERAGE(D4:D10)</f>
         <v>35219.714285714283</v>
       </c>
-      <c r="E11" s="10">
+      <c r="E11" s="7">
         <f>AVERAGE(E4:E9)</f>
         <v>11277.333333333334</v>
       </c>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="D13" s="10">
-        <f>SUM(C11:E11)</f>
-        <v>47303.476190476191</v>
+      <c r="D13" s="7">
+        <f>SUM(D11:E11)</f>
+        <v>46497.047619047618</v>
+      </c>
+    </row>
+    <row r="18" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D18">
+        <v>37900</v>
+      </c>
+      <c r="E18">
+        <v>8978</v>
       </c>
     </row>
   </sheetData>
@@ -757,5 +803,6 @@
     <mergeCell ref="G2:I2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>